<commit_message>
Version of deploy 0.614 from 27.03.2025. Import barcodes
</commit_message>
<xml_diff>
--- a/downloads/import_offers_tmp.xlsx
+++ b/downloads/import_offers_tmp.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>of_sku</t>
   </si>
@@ -22,6 +22,9 @@
     <t>of_name</t>
   </si>
   <si>
+    <t>of_barcode</t>
+  </si>
+  <si>
     <t>of_price</t>
   </si>
   <si>
@@ -32,6 +35,9 @@
   </si>
   <si>
     <t>Brainstring Advanced 2.0</t>
+  </si>
+  <si>
+    <t>2003357847234</t>
   </si>
   <si>
     <r>
@@ -48,6 +54,9 @@
     <t>MindJewel</t>
   </si>
   <si>
+    <t>2005847345742,23445542345</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -62,6 +71,9 @@
     <t>IcoSoKu</t>
   </si>
   <si>
+    <t>3453453466544</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -91,6 +103,9 @@
   </si>
   <si>
     <t>3D Crystal Puzzles Apple</t>
+  </si>
+  <si>
+    <t>3453455667777</t>
   </si>
   <si>
     <r>
@@ -172,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -285,13 +300,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -335,6 +437,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -360,6 +489,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1391,18 +1521,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="4" width="31.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.15" customHeight="1">
@@ -1421,97 +1551,149 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s" s="5">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="F2" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="D3" s="11">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="E3" s="11">
         <v>20</v>
       </c>
-      <c r="E3" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="F3" s="12"/>
+      <c r="F3" t="s" s="10">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="E4" s="11">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="10">
-        <v>11</v>
-      </c>
-      <c r="F4" s="12"/>
+      <c r="F4" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="D5" s="11">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11">
         <v>8.5</v>
       </c>
-      <c r="E5" t="s" s="10">
-        <v>13</v>
-      </c>
-      <c r="F5" s="12"/>
+      <c r="F5" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D6" s="11">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="E6" s="11">
         <v>6</v>
       </c>
-      <c r="E6" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="F6" s="12"/>
+      <c r="F6" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" ht="14.7" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display="https://nwms.cloud/upload/catalog/Uzel_2.jpg"/>
-    <hyperlink ref="E3" r:id="rId2" location="" tooltip="" display="https://nwms.cloud/upload/catalog/Izumrud.jpg"/>
-    <hyperlink ref="E4" r:id="rId3" location="" tooltip="" display="https://nwms.cloud/upload/catalog/Sudoku-SHar.jpg"/>
-    <hyperlink ref="E5" r:id="rId4" location="" tooltip="" display="https://nwms.cloud/upload/catalog/SHarik_Rubika.jpg"/>
-    <hyperlink ref="E6" r:id="rId5" location="" tooltip="" display="https://nwms.cloud/upload/catalog/YAbloko.jpg"/>
+    <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="https://nwms.cloud/upload/catalog/Uzel_2.jpg"/>
+    <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="https://nwms.cloud/upload/catalog/Izumrud.jpg"/>
+    <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="https://nwms.cloud/upload/catalog/Sudoku-SHar.jpg"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="https://nwms.cloud/upload/catalog/SHarik_Rubika.jpg"/>
+    <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="https://nwms.cloud/upload/catalog/YAbloko.jpg"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>